<commit_message>
cambios subir periodos como admin
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Pdfs_ejemplos_periodos_anteriores.xlsx
+++ b/app/dataextraction/Recibos/Pdfs_ejemplos_periodos_anteriores.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26E0212-EA54-4804-ADD4-E3CFA4B47FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09578E78-347F-4D60-B6CE-78E02198FA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60557611-8CDE-40A3-9DB6-3888F4CD0DFF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{60557611-8CDE-40A3-9DB6-3888F4CD0DFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="FechasCalendario" sheetId="2" r:id="rId1"/>
-    <sheet name="Clientes" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="FechasCalendario" sheetId="2" r:id="rId2"/>
+    <sheet name="Clientes" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FechasCalendario!$A$1:$M$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FechasCalendario!$A$1:$M$57</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="40">
-  <si>
-    <t>pais</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="44">
   <si>
     <t>id_razonsocial</t>
   </si>
@@ -147,16 +148,31 @@
     <t>Flor Cardenas</t>
   </si>
   <si>
-    <t>Juan Expinosa</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Pendiente</t>
   </si>
   <si>
     <t xml:space="preserve"> año</t>
+  </si>
+  <si>
+    <t>Camilo Sarmiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; </t>
+  </si>
+  <si>
+    <t>Juan Espinosa</t>
+  </si>
+  <si>
+    <t>Maria Rivera</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of id_razonsocial</t>
   </si>
 </sst>
 </file>
@@ -232,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,6 +301,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,6 +321,516 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="jazmin pineda" refreshedDate="44884.761756481479" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="68" xr:uid="{173BED8B-FE3B-4454-AB3B-A68F59880A27}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:D57" sheet="FechasCalendario"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="id_razonsocial" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="9002144587" maxValue="9302112487"/>
+    </cacheField>
+    <cacheField name="nombre_empresa" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="periodo_fiscal" numFmtId="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="8" count="6">
+        <n v="4"/>
+        <n v="3"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name=" año" numFmtId="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2022" maxValue="2022"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="68">
+  <r>
+    <s v="30-70892838-7"/>
+    <s v="BSF SA"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002185787"/>
+    <s v="SISTEMAS COLOMBIA S.A.S"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI620328DP8"/>
+    <s v="NCS PEARSON, INC."/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9013543905"/>
+    <s v="AIRBNB IRELAND UNLIMITED COMPANY"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-70892838-7"/>
+    <s v="BSF SA"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002185787"/>
+    <s v="SISTEMAS COLOMBIA S.A.S"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI620328DP8"/>
+    <s v="NCS PEARSON, INC."/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9013543905"/>
+    <s v="AIRBNB IRELAND UNLIMITED COMPANY"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-71245283-4"/>
+    <s v="DYNAFLOWS SA"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-71245283-4"/>
+    <s v="DYNAFLOWS SA"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002145787"/>
+    <s v="INVERSIONES ELENA COLOMBIA S.A.S"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002145787"/>
+    <s v="INVERSIONES ELENA COLOMBIA S.A.S"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI645328DP8"/>
+    <s v="DECORIET, INC."/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI645328DP8"/>
+    <s v="DECORIET, INC."/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71565283-4"/>
+    <s v="INVERSIONES FLORXS SA"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71565283-4"/>
+    <s v="INVERSIONES FLORXS SA"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9302112487"/>
+    <s v="ELPEHMB SAS"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9302112487"/>
+    <s v="ELPEHMB SAS"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="N45645458DP8"/>
+    <s v="LA TOSCANA LITD"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="N45645458DP8"/>
+    <s v="LA TOSCANA LITD"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002144587"/>
+    <s v="PASS CLASS SAS"/>
+    <x v="0"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002144587"/>
+    <s v="PASS CLASS SAS"/>
+    <x v="1"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-70892838-7"/>
+    <s v="BSF SA"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002185787"/>
+    <s v="SISTEMAS COLOMBIA S.A.S"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI620328DP8"/>
+    <s v="NCS PEARSON, INC."/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9013543905"/>
+    <s v="AIRBNB IRELAND UNLIMITED COMPANY"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-71245283-4"/>
+    <s v="DYNAFLOWS SA"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002145787"/>
+    <s v="INVERSIONES ELENA COLOMBIA S.A.S"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI645328DP8"/>
+    <s v="DECORIET, INC."/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71565283-4"/>
+    <s v="INVERSIONES FLORXS SA"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9302112487"/>
+    <s v="ELPEHMB SAS"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="N45645458DP8"/>
+    <s v="LA TOSCANA LITD"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002144587"/>
+    <s v="PASS CLASS SAS"/>
+    <x v="2"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-70892838-7"/>
+    <s v="BSF SA"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002185787"/>
+    <s v="SISTEMAS COLOMBIA S.A.S"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI620328DP8"/>
+    <s v="NCS PEARSON, INC."/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9013543905"/>
+    <s v="AIRBNB IRELAND UNLIMITED COMPANY"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-71245283-4"/>
+    <s v="DYNAFLOWS SA"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002145787"/>
+    <s v="INVERSIONES ELENA COLOMBIA S.A.S"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI645328DP8"/>
+    <s v="DECORIET, INC."/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71565283-4"/>
+    <s v="INVERSIONES FLORXS SA"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9302112487"/>
+    <s v="ELPEHMB SAS"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="N45645458DP8"/>
+    <s v="LA TOSCANA LITD"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002144587"/>
+    <s v="PASS CLASS SAS"/>
+    <x v="3"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-70892838-7"/>
+    <s v="BSF SA"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002185787"/>
+    <s v="SISTEMAS COLOMBIA S.A.S"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI620328DP8"/>
+    <s v="NCS PEARSON, INC."/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9013543905"/>
+    <s v="AIRBNB IRELAND UNLIMITED COMPANY"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002145787"/>
+    <s v="INVERSIONES ELENA COLOMBIA S.A.S"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI645328DP8"/>
+    <s v="DECORIET, INC."/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71565283-4"/>
+    <s v="INVERSIONES FLORXS SA"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9302112487"/>
+    <s v="ELPEHMB SAS"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="N45645458DP8"/>
+    <s v="LA TOSCANA LITD"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71244583-4"/>
+    <s v="FACUNDOS Y COMPAÑIA SA"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002144587"/>
+    <s v="PASS CLASS SAS"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI456458DP8"/>
+    <s v="EMERSON E INVERTNSO LITD"/>
+    <x v="4"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="30-70892838-7"/>
+    <s v="BSF SA"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002185787"/>
+    <s v="SISTEMAS COLOMBIA S.A.S"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI620328DP8"/>
+    <s v="NCS PEARSON, INC."/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9013543905"/>
+    <s v="AIRBNB IRELAND UNLIMITED COMPANY"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002145787"/>
+    <s v="INVERSIONES ELENA COLOMBIA S.A.S"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI645328DP8"/>
+    <s v="DECORIET, INC."/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71565283-4"/>
+    <s v="INVERSIONES FLORXS SA"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9302112487"/>
+    <s v="ELPEHMB SAS"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="N45645458DP8"/>
+    <s v="LA TOSCANA LITD"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="31-71244583-4"/>
+    <s v="FACUNDOS Y COMPAÑIA SA"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <n v="9002144587"/>
+    <s v="PASS CLASS SAS"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+  <r>
+    <s v="NPI456458DP8"/>
+    <s v="EMERSON E INVERTNSO LITD"/>
+    <x v="5"/>
+    <n v="2022"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F10EB4D-7D00-4142-A35A-F516DE52E0FB}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="1" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of id_razonsocial" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,11 +1129,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA9833F-BC39-4A1F-B455-234304473A55}">
+  <dimension ref="A3:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="27">
+        <v>6</v>
+      </c>
+      <c r="B7" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="27">
+        <v>8</v>
+      </c>
+      <c r="B9" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="28">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E8BB8A-DBEC-4B54-AB25-2A70177B11AD}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,43 +1232,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
       <c r="I1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>34</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="21">
         <v>4</v>
@@ -667,19 +1281,19 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="24">
         <v>44691</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -687,7 +1301,7 @@
         <v>9002185787</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="21">
         <v>4</v>
@@ -700,27 +1314,27 @@
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="24">
         <v>44695</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="21">
         <v>4</v>
@@ -733,19 +1347,19 @@
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="I4" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="24">
         <v>44699</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -753,7 +1367,7 @@
         <v>9013543905</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="21">
         <v>4</v>
@@ -766,27 +1380,27 @@
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K5" s="24">
         <v>44699</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="21">
         <v>3</v>
@@ -799,19 +1413,19 @@
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="24">
         <v>44661</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -819,7 +1433,7 @@
         <v>9002185787</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="21">
         <v>3</v>
@@ -832,27 +1446,27 @@
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K7" s="24">
         <v>44665</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>13</v>
       </c>
       <c r="C8" s="21">
         <v>3</v>
@@ -865,19 +1479,19 @@
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K8" s="24">
         <v>44669</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -885,7 +1499,7 @@
         <v>9013543905</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="21">
         <v>3</v>
@@ -898,27 +1512,27 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" s="24">
         <v>44669</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>10</v>
       </c>
       <c r="C10" s="21">
         <v>4</v>
@@ -931,27 +1545,27 @@
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K10" s="24">
         <v>44699</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>9</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>10</v>
       </c>
       <c r="C11" s="21">
         <v>3</v>
@@ -964,19 +1578,19 @@
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K11" s="24">
         <v>44661</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -984,7 +1598,7 @@
         <v>9002145787</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="21">
         <v>4</v>
@@ -997,19 +1611,19 @@
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="24">
         <v>44699</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -1017,7 +1631,7 @@
         <v>9002145787</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="21">
         <v>3</v>
@@ -1030,27 +1644,27 @@
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" s="24">
         <v>44665</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>17</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>18</v>
       </c>
       <c r="C14" s="21">
         <v>4</v>
@@ -1063,27 +1677,27 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K14" s="24">
         <v>44699</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>17</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>18</v>
       </c>
       <c r="C15" s="21">
         <v>3</v>
@@ -1096,27 +1710,27 @@
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K15" s="24">
         <v>44669</v>
       </c>
       <c r="L15" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="21">
         <v>4</v>
@@ -1129,27 +1743,27 @@
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
       <c r="I16" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K16" s="24">
         <v>44699</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="21">
         <v>3</v>
@@ -1162,19 +1776,19 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K17" s="24">
         <v>44661</v>
       </c>
       <c r="L17" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -1182,7 +1796,7 @@
         <v>9302112487</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="21">
         <v>4</v>
@@ -1195,19 +1809,19 @@
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K18" s="24">
         <v>44699</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -1215,7 +1829,7 @@
         <v>9302112487</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="21">
         <v>3</v>
@@ -1228,27 +1842,27 @@
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K19" s="24">
         <v>44665</v>
       </c>
       <c r="L19" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="21">
         <v>4</v>
@@ -1261,27 +1875,27 @@
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K20" s="24">
         <v>44699</v>
       </c>
-      <c r="L20" s="24" t="s">
-        <v>36</v>
+      <c r="L20" t="s">
+        <v>40</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="21">
         <v>3</v>
@@ -1294,27 +1908,27 @@
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K21" s="24">
         <v>44669</v>
       </c>
-      <c r="L21" s="24" t="s">
-        <v>36</v>
+      <c r="L21" t="s">
+        <v>40</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="19">
+        <v>9002144587</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>23</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>22</v>
       </c>
       <c r="C22" s="21">
         <v>4</v>
@@ -1327,7 +1941,7 @@
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J22" s="23" t="s">
         <v>30</v>
@@ -1336,18 +1950,18 @@
         <v>44699</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="19">
+        <v>9002144587</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>23</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>22</v>
       </c>
       <c r="C23" s="21">
         <v>3</v>
@@ -1360,30 +1974,30 @@
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
       <c r="I23" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J23" s="23" t="s">
         <v>30</v>
       </c>
       <c r="K23" s="24">
-        <v>44661</v>
+        <v>44665</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
-        <v>9002144587</v>
+      <c r="A24" s="19" t="s">
+        <v>5</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C24" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" s="21">
         <v>2022</v>
@@ -1393,30 +2007,30 @@
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
       <c r="I24" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K24" s="24">
-        <v>44699</v>
+        <v>44722</v>
       </c>
       <c r="L24" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
-        <v>9002144587</v>
+        <v>9002185787</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C25" s="21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="21">
         <v>2022</v>
@@ -1426,30 +2040,30 @@
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K25" s="24">
-        <v>44665</v>
+        <v>44726</v>
       </c>
       <c r="L25" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M25" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="M25" s="22" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C26" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" s="21">
         <v>2022</v>
@@ -1459,30 +2073,30 @@
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="24">
+        <v>44730</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="19">
+        <v>9013543905</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="24">
-        <v>44699</v>
-      </c>
-      <c r="L26" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M26" s="22" t="s">
+      <c r="C27" s="21">
         <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="21">
-        <v>3</v>
       </c>
       <c r="D27" s="21">
         <v>2022</v>
@@ -1492,27 +2106,27 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="22" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K27" s="24">
-        <v>44669</v>
+        <v>44730</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19" t="s">
-        <v>6</v>
+      <c r="A28" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C28" s="21">
         <v>5</v>
@@ -1525,27 +2139,27 @@
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K28" s="24">
-        <v>44722</v>
+        <v>44730</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
-        <v>9002185787</v>
+        <v>9002145787</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C29" s="21">
         <v>5</v>
@@ -1558,27 +2172,27 @@
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
       <c r="I29" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K29" s="24">
-        <v>44726</v>
+        <v>44730</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C30" s="21">
         <v>5</v>
@@ -1591,27 +2205,27 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K30" s="24">
         <v>44730</v>
       </c>
       <c r="L30" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M30" s="22" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19">
-        <v>9013543905</v>
+      <c r="A31" s="25" t="s">
+        <v>25</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C31" s="21">
         <v>5</v>
@@ -1624,27 +2238,27 @@
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
       <c r="I31" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K31" s="24">
         <v>44730</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25" t="s">
-        <v>9</v>
+      <c r="A32" s="19">
+        <v>9302112487</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C32" s="21">
         <v>5</v>
@@ -1657,7 +2271,7 @@
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
       <c r="I32" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J32" s="23" t="s">
         <v>30</v>
@@ -1666,18 +2280,18 @@
         <v>44730</v>
       </c>
       <c r="L32" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M32" s="22" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19">
-        <v>9002145787</v>
+      <c r="A33" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C33" s="21">
         <v>5</v>
@@ -1690,7 +2304,7 @@
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
       <c r="I33" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J33" s="23" t="s">
         <v>31</v>
@@ -1698,19 +2312,19 @@
       <c r="K33" s="24">
         <v>44730</v>
       </c>
-      <c r="L33" s="24" t="s">
-        <v>36</v>
+      <c r="L33" t="s">
+        <v>40</v>
       </c>
       <c r="M33" s="22" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19" t="s">
-        <v>17</v>
+      <c r="A34" s="19">
+        <v>9002144587</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C34" s="21">
         <v>5</v>
@@ -1723,30 +2337,30 @@
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="22" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K34" s="24">
         <v>44730</v>
       </c>
       <c r="L34" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M34" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
-        <v>26</v>
-      </c>
       <c r="B35" s="20" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C35" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D35" s="21">
         <v>2022</v>
@@ -1756,30 +2370,30 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K35" s="24">
-        <v>44730</v>
+        <v>44752</v>
       </c>
       <c r="L35" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M35" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="M35" s="22" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
-        <v>9302112487</v>
+        <v>9002185787</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C36" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D36" s="21">
         <v>2022</v>
@@ -1789,30 +2403,30 @@
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="I36" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K36" s="24">
-        <v>44730</v>
+        <v>44756</v>
       </c>
       <c r="L36" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M36" s="22" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C37" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D37" s="21">
         <v>2022</v>
@@ -1822,30 +2436,30 @@
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="I37" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K37" s="24">
+        <v>44760</v>
+      </c>
+      <c r="L37" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M37" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="19">
+        <v>9013543905</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J37" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="K37" s="24">
-        <v>44730</v>
-      </c>
-      <c r="L37" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="M37" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>22</v>
-      </c>
       <c r="C38" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D38" s="21">
         <v>2022</v>
@@ -1855,30 +2469,30 @@
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J38" s="23" t="s">
         <v>30</v>
       </c>
       <c r="K38" s="24">
-        <v>44730</v>
+        <v>44760</v>
       </c>
       <c r="L38" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M38" s="22" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="19">
-        <v>9002144587</v>
+      <c r="A39" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C39" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D39" s="21">
         <v>2022</v>
@@ -1888,30 +2502,30 @@
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
       <c r="I39" s="22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K39" s="24">
-        <v>44730</v>
+        <v>44760</v>
       </c>
       <c r="L39" s="24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="M39" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>25</v>
+      <c r="A40" s="19">
+        <v>9002145787</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C40" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D40" s="21">
         <v>2022</v>
@@ -1921,29 +2535,589 @@
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
       <c r="I40" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="24">
+        <v>44760</v>
+      </c>
+      <c r="L40" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M40" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="21">
+        <v>6</v>
+      </c>
+      <c r="D41" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K41" s="24">
+        <v>44760</v>
+      </c>
+      <c r="L41" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M41" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="21">
+        <v>6</v>
+      </c>
+      <c r="D42" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K42" s="24">
+        <v>44760</v>
+      </c>
+      <c r="L42" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M42" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="19">
+        <v>9302112487</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="21">
+        <v>6</v>
+      </c>
+      <c r="D43" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K43" s="24">
+        <v>44760</v>
+      </c>
+      <c r="L43" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M43" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="21">
+        <v>6</v>
+      </c>
+      <c r="D44" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K44" s="24">
+        <v>44760</v>
+      </c>
+      <c r="L44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M44" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="19">
+        <v>9002144587</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="21">
+        <v>6</v>
+      </c>
+      <c r="D45" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K45" s="24">
+        <v>44760</v>
+      </c>
+      <c r="L45" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M45" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="21">
+        <v>7</v>
+      </c>
+      <c r="D46" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K46" s="24">
+        <v>44783</v>
+      </c>
+      <c r="L46" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M46" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="19">
+        <v>9002185787</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="21">
+        <v>7</v>
+      </c>
+      <c r="D47" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K47" s="24">
+        <v>44787</v>
+      </c>
+      <c r="L47" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M47" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="21">
+        <v>7</v>
+      </c>
+      <c r="D48" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L48" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M48" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="19">
+        <v>9013543905</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J40" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="K40" s="24">
-        <v>44730</v>
-      </c>
-      <c r="L40" s="24" t="s">
+      <c r="C49" s="21">
+        <v>7</v>
+      </c>
+      <c r="D49" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K49" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L49" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M49" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="19">
+        <v>9002145787</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="21">
+        <v>7</v>
+      </c>
+      <c r="D50" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K50" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L50" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M50" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="21">
+        <v>7</v>
+      </c>
+      <c r="D51" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K51" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L51" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M51" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="21">
+        <v>7</v>
+      </c>
+      <c r="D52" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K52" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L52" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M52" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="M40" s="22" t="s">
-        <v>5</v>
+    </row>
+    <row r="53" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="19">
+        <v>9302112487</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="21">
+        <v>7</v>
+      </c>
+      <c r="D53" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K53" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L53" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M53" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="21">
+        <v>7</v>
+      </c>
+      <c r="D54" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K54" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L54" t="s">
+        <v>40</v>
+      </c>
+      <c r="M54" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="21">
+        <v>7</v>
+      </c>
+      <c r="D55" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K55" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L55" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M55" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="19">
+        <v>9002144587</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="21">
+        <v>7</v>
+      </c>
+      <c r="D56" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K56" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L56" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M56" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="21">
+        <v>7</v>
+      </c>
+      <c r="D57" s="21">
+        <v>2022</v>
+      </c>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K57" s="24">
+        <v>44791</v>
+      </c>
+      <c r="L57" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M57" s="22" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M40" xr:uid="{83E8BB8A-DBEC-4B54-AB25-2A70177B11AD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2192205D-4D26-4639-8663-BD635BDD14CC}">
   <dimension ref="A1:B35"/>
   <sheetViews>
@@ -1959,18 +3133,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1978,15 +3152,15 @@
         <v>9002185787</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1994,15 +3168,15 @@
         <v>9013543905</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2010,23 +3184,23 @@
         <v>9002145787</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2034,23 +3208,23 @@
         <v>9302112487</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2058,15 +3232,15 @@
         <v>9002144587</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>